<commit_message>
separate polygon and point columns
</commit_message>
<xml_diff>
--- a/inputs/lsib_extension/adm0_lines.xlsx
+++ b/inputs/lsib_extension/adm0_lines.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/computer/GitHub/fieldmaps/adm0-generator/inputs/lsib_extension/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{344D9851-430F-0D4D-A038-E53CD85DE0C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35B65818-177F-C34C-A555-95619CEDD632}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20560" yWindow="880" windowWidth="20560" windowHeight="25700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="880" windowWidth="41120" windowHeight="25700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="adm0_lines" sheetId="1" r:id="rId1"/>
@@ -1661,9 +1661,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N409"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A335" workbookViewId="0">
-      <selection activeCell="E159" sqref="E159"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>

</xml_diff>